<commit_message>
Refatorado para somar os pesos
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CLJ1276</t>
+          <t>CJL1276</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -461,7 +461,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12330</t>
+          <t>42000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>19/04/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CJL1276</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>35000</t>
         </is>
       </c>
     </row>

</xml_diff>